<commit_message>
add all employers and tasks
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,922 +511,922 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Аниськина Е.А.</t>
+          <t>Аггеев Д.А.</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>51</v>
+        <v>47.75</v>
       </c>
       <c r="D4" t="n">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="E4" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Афанасьева Н.В.</t>
+          <t>Акимов В.И.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>71</v>
+        <v>40.2</v>
       </c>
       <c r="D5" t="n">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E5" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Белоусова Е,В.</t>
+          <t>Акульшин А.П.</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>66.66666666666667</v>
+        <v>47.4</v>
       </c>
       <c r="D6" t="n">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="E6" t="n">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Бодров О.В.</t>
+          <t>Алексеев А.Г.</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>37.33333333333334</v>
+        <v>54.33333333333334</v>
       </c>
       <c r="D7" t="n">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="F7" t="n">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Болвачева И. А.</t>
+          <t>Андрианов С.Д,</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>223</v>
+      </c>
+      <c r="E8" t="n">
+        <v>37</v>
+      </c>
+      <c r="F8" t="n">
         <v>63</v>
-      </c>
-      <c r="D8" t="n">
-        <v>189</v>
-      </c>
-      <c r="E8" t="n">
-        <v>49</v>
-      </c>
-      <c r="F8" t="n">
-        <v>76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Борисов А.Ю.</t>
+          <t>Аниськина Е.А.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D9" t="n">
-        <v>108</v>
+        <v>204</v>
       </c>
       <c r="E9" t="n">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F9" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Бубнова Е.В.</t>
+          <t>Арзамасцев В.В.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>61.33333333333334</v>
+        <v>62</v>
       </c>
       <c r="D10" t="n">
-        <v>184</v>
+        <v>62</v>
       </c>
       <c r="E10" t="n">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="F10" t="n">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Будников А.В.</t>
+          <t>Афанасьева Н.В.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D11" t="n">
-        <v>54</v>
+        <v>213</v>
       </c>
       <c r="E11" t="n">
         <v>54</v>
       </c>
       <c r="F11" t="n">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Бушуев А.А.</t>
+          <t>Бабенков А. А.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
+        <v>45.16666666666666</v>
+      </c>
+      <c r="D12" t="n">
+        <v>271</v>
+      </c>
+      <c r="E12" t="n">
+        <v>36</v>
+      </c>
+      <c r="F12" t="n">
         <v>54</v>
-      </c>
-      <c r="D12" t="n">
-        <v>108</v>
-      </c>
-      <c r="E12" t="n">
-        <v>53</v>
-      </c>
-      <c r="F12" t="n">
-        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Гавриленко О.В.</t>
+          <t>Белоусова Е,В.</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>54</v>
+        <v>66.66666666666667</v>
       </c>
       <c r="D13" t="n">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="E13" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="n">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Горохова Е.Н.</t>
+          <t>Билжа С.Й</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>52.25</v>
+        <v>47.4</v>
       </c>
       <c r="D14" t="n">
-        <v>209</v>
+        <v>237</v>
       </c>
       <c r="E14" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F14" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Гусева Н.И.</t>
+          <t>Бодров О.В.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D15" t="n">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="E15" t="n">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F15" t="n">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Жукова Г.Б.</t>
+          <t>Болвачева И. А.</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>64.33333333333333</v>
+        <v>63</v>
       </c>
       <c r="D16" t="n">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E16" t="n">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F16" t="n">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Захарова К.Г.</t>
+          <t>Борисов А.Ю.</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>70</v>
+        <v>44.25</v>
       </c>
       <c r="D17" t="n">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="E17" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F17" t="n">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Инкин Г.А.</t>
+          <t>Боталов А.М.</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>41</v>
+        <v>50.4</v>
       </c>
       <c r="D18" t="n">
-        <v>123</v>
+        <v>252</v>
       </c>
       <c r="E18" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F18" t="n">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Исаева Э.Е.</t>
+          <t>Бубнова Е.В.</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>47.33333333333334</v>
+        <v>61.33333333333334</v>
       </c>
       <c r="D19" t="n">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="E19" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Карева Т.Ю.</t>
+          <t>Будников А.В.</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>70.33333333333333</v>
+        <v>43</v>
       </c>
       <c r="D20" t="n">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="E20" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F20" t="n">
-        <v>108</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Киселева Н.В.</t>
+          <t>Бушуев А.А.</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>52</v>
+        <v>49.2</v>
       </c>
       <c r="D21" t="n">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="E21" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F21" t="n">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Ковалева Ю.Г.</t>
+          <t>Быков Е.А.</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>50</v>
+        <v>45.16666666666666</v>
       </c>
       <c r="D22" t="n">
-        <v>200</v>
+        <v>271</v>
       </c>
       <c r="E22" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F22" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Козлова Е. В.</t>
+          <t>Викторов В.В.</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>67.66666666666667</v>
+        <v>48.4</v>
       </c>
       <c r="D23" t="n">
-        <v>203</v>
+        <v>242</v>
       </c>
       <c r="E23" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F23" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Колесникова Е,И.</t>
+          <t>Воробьёв С.В.</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>80</v>
+        <v>47.2</v>
       </c>
       <c r="D24" t="n">
-        <v>160</v>
+        <v>236</v>
       </c>
       <c r="E24" t="n">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="F24" t="n">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Кольцов М.Ю.</t>
+          <t>Гавриленко О.В.</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>42</v>
+        <v>50.6</v>
       </c>
       <c r="D25" t="n">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="E25" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25" t="n">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Кондратенко А.Н.</t>
+          <t>Герасименко А.Т.</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D26" t="n">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="E26" t="n">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Кузнецов Е.Б.</t>
+          <t>Горностаев И.Б.</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>64.5</v>
+        <v>41.8</v>
       </c>
       <c r="D27" t="n">
-        <v>129</v>
+        <v>209</v>
       </c>
       <c r="E27" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F27" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Куклина Ф.Н.</t>
+          <t>Горохова Е.Н.</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>38</v>
+        <v>52.25</v>
       </c>
       <c r="D28" t="n">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="E28" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F28" t="n">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Курочкина И.В.</t>
+          <t>Гусева Н.И.</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>64.66666666666667</v>
+        <v>66</v>
       </c>
       <c r="D29" t="n">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E29" t="n">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F29" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Лазутин Д.В.</t>
+          <t>Демидов А.С.</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>42</v>
+        <v>50.8</v>
       </c>
       <c r="D30" t="n">
-        <v>84</v>
+        <v>254</v>
       </c>
       <c r="E30" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F30" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Лобова Е.В.</t>
+          <t>Дядищев С.В.</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>69.66666666666667</v>
+        <v>44</v>
       </c>
       <c r="D31" t="n">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="E31" t="n">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F31" t="n">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Мазеин А.П.</t>
+          <t>Ефремов П.С,</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C32" t="n">
-        <v>42</v>
+        <v>45.33333333333334</v>
       </c>
       <c r="D32" t="n">
-        <v>84</v>
+        <v>272</v>
       </c>
       <c r="E32" t="n">
         <v>30</v>
       </c>
       <c r="F32" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Макарова А.С.</t>
+          <t>Жукова Г.Б.</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>61.66666666666666</v>
+        <v>64.33333333333333</v>
       </c>
       <c r="D33" t="n">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E33" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F33" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Марухина Н.А.</t>
+          <t>Захаров Д.И.</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D34" t="n">
-        <v>58</v>
+        <v>230</v>
       </c>
       <c r="E34" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F34" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Минкина Е.К.</t>
+          <t>Захарова К.Г.</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>62.66666666666666</v>
+        <v>70</v>
       </c>
       <c r="D35" t="n">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="E35" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F35" t="n">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Миронова Л.В.</t>
+          <t>Зиновьев С.В.</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>48</v>
+        <v>44.33333333333334</v>
       </c>
       <c r="D36" t="n">
-        <v>48</v>
+        <v>266</v>
       </c>
       <c r="E36" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F36" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Неустроева С.В.</t>
+          <t>Инкин Г.А.</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C37" t="n">
-        <v>70.33333333333333</v>
+        <v>38.33333333333334</v>
       </c>
       <c r="D37" t="n">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="E37" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F37" t="n">
-        <v>110</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Нехаев А.В.</t>
+          <t>Исаев М.М.</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>50.25</v>
+        <v>50.75</v>
       </c>
       <c r="D38" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E38" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F38" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Новожилов С.В.</t>
+          <t>Исаева Э.Е.</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>53</v>
+        <v>47.33333333333334</v>
       </c>
       <c r="D39" t="n">
-        <v>212</v>
+        <v>142</v>
       </c>
       <c r="E39" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F39" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Носова А.А.</t>
+          <t>Карева Т.Ю.</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>3</v>
       </c>
       <c r="C40" t="n">
-        <v>66.33333333333333</v>
+        <v>70.33333333333333</v>
       </c>
       <c r="D40" t="n">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="E40" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F40" t="n">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Першин А.А.</t>
+          <t>Киселева Н.В.</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
+        <v>52</v>
+      </c>
+      <c r="D41" t="n">
+        <v>208</v>
+      </c>
+      <c r="E41" t="n">
         <v>41</v>
       </c>
-      <c r="D41" t="n">
-        <v>123</v>
-      </c>
-      <c r="E41" t="n">
-        <v>25</v>
-      </c>
       <c r="F41" t="n">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Пилатова А.Е. </t>
+          <t>Кобзев Д.В.</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
-        <v>51.25</v>
+        <v>50.6</v>
       </c>
       <c r="D42" t="n">
-        <v>205</v>
+        <v>253</v>
       </c>
       <c r="E42" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>56</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Ратникова Т.И.</t>
+          <t>Ковалева Ю.Г.</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>51.25</v>
+        <v>50</v>
       </c>
       <c r="D43" t="n">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E43" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F43" t="n">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Сажнева О.В.</t>
+          <t>Коваленко А.В.</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>68.33333333333333</v>
+        <v>40.8</v>
       </c>
       <c r="D44" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44" t="n">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="F44" t="n">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Силаева О.И.</t>
+          <t>Козлова Е. В.</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>70.33333333333333</v>
+        <v>67.66666666666667</v>
       </c>
       <c r="D45" t="n">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E45" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F45" t="n">
         <v>77</v>
@@ -1435,64 +1435,64 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Смирнова О.В.</t>
+          <t>Колесникова Е,И.</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C46" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D46" t="n">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="E46" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F46" t="n">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Солодовникова Н.В.</t>
+          <t>Колобков К.М</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>55.66666666666666</v>
+        <v>40.6</v>
       </c>
       <c r="D47" t="n">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="E47" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F47" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Столярова И.В.</t>
+          <t>Кольцов М.Ю.</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>60.33333333333334</v>
+        <v>49.2</v>
       </c>
       <c r="D48" t="n">
-        <v>181</v>
+        <v>246</v>
       </c>
       <c r="E48" t="n">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F48" t="n">
         <v>65</v>
@@ -1501,331 +1501,1431 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Таковникова Н.А.</t>
+          <t>Кондратенко А.Н.</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>71.5</v>
+        <v>72</v>
       </c>
       <c r="D49" t="n">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="E49" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F49" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Тарасова Ю.П.</t>
+          <t>Корнеев К.В.</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>67</v>
+        <v>47.2</v>
       </c>
       <c r="D50" t="n">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="E50" t="n">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F50" t="n">
-        <v>90</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Теленкова В.А.</t>
+          <t>Костин В.Ю.</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>106.5</v>
+        <v>49.4</v>
       </c>
       <c r="D51" t="n">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="E51" t="n">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="F51" t="n">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Тихомирова Е.Е.</t>
+          <t>Костюков Н.В.</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>70.66666666666667</v>
+        <v>42.8</v>
       </c>
       <c r="D52" t="n">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E52" t="n">
+        <v>36</v>
+      </c>
+      <c r="F52" t="n">
         <v>52</v>
-      </c>
-      <c r="F52" t="n">
-        <v>91</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Тришкина Е.В.</t>
+          <t xml:space="preserve">Кузнецов А.В. </t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C53" t="n">
-        <v>65</v>
+        <v>45.33333333333334</v>
       </c>
       <c r="D53" t="n">
-        <v>130</v>
+        <v>272</v>
       </c>
       <c r="E53" t="n">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="F53" t="n">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Тушинок С.Н.</t>
+          <t>Кузнецов Е.Б.</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="n">
-        <v>57.33333333333334</v>
+        <v>64.5</v>
       </c>
       <c r="D54" t="n">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="E54" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F54" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Удовенко М.С.</t>
+          <t>Куклина Ф.Н.</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>43.25</v>
+        <v>38</v>
       </c>
       <c r="D55" t="n">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="E55" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F55" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Фокина Е.А.</t>
+          <t>Курочкина И.В.</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" t="n">
-        <v>49.25</v>
+        <v>64.66666666666667</v>
       </c>
       <c r="D56" t="n">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E56" t="n">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F56" t="n">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Хализев В.И.</t>
+          <t>Лазутин Д.В.</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C57" t="n">
-        <v>46</v>
+        <v>41.33333333333334</v>
       </c>
       <c r="D57" t="n">
-        <v>46</v>
+        <v>248</v>
       </c>
       <c r="E57" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F57" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Ходченкова М.Н.</t>
+          <t>Лобова Е.В.</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>3</v>
       </c>
       <c r="C58" t="n">
-        <v>62.33333333333334</v>
+        <v>69.66666666666667</v>
       </c>
       <c r="D58" t="n">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="E58" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F58" t="n">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Христофорова О.С.</t>
+          <t>Лыков К.А.</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C59" t="n">
-        <v>53.66666666666666</v>
+        <v>41.2</v>
       </c>
       <c r="D59" t="n">
-        <v>161</v>
+        <v>206</v>
       </c>
       <c r="E59" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F59" t="n">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Чернявская В.А.</t>
+          <t>Мазеин А.П.</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" t="n">
-        <v>51.25</v>
+        <v>51.2</v>
       </c>
       <c r="D60" t="n">
-        <v>205</v>
+        <v>256</v>
       </c>
       <c r="E60" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F60" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Шварева М.В.</t>
+          <t>Макарова А.С.</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61" t="n">
-        <v>50</v>
+        <v>61.66666666666666</v>
       </c>
       <c r="D61" t="n">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="E61" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F61" t="n">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Шувалова Т.А.</t>
+          <t>Марухина Н.А.</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>42.2</v>
+        <v>58</v>
       </c>
       <c r="D62" t="n">
-        <v>211</v>
+        <v>58</v>
       </c>
       <c r="E62" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="F62" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
+          <t>Медведев П.С.</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>46</v>
+      </c>
+      <c r="D63" t="n">
+        <v>230</v>
+      </c>
+      <c r="E63" t="n">
+        <v>30</v>
+      </c>
+      <c r="F63" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>Минкина Е.К.</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" t="n">
+        <v>62.66666666666666</v>
+      </c>
+      <c r="D64" t="n">
+        <v>188</v>
+      </c>
+      <c r="E64" t="n">
+        <v>43</v>
+      </c>
+      <c r="F64" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>Миронова Л.В.</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>48</v>
+      </c>
+      <c r="D65" t="n">
+        <v>48</v>
+      </c>
+      <c r="E65" t="n">
+        <v>48</v>
+      </c>
+      <c r="F65" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Мурзак Д.Г.</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="D66" t="n">
+        <v>243</v>
+      </c>
+      <c r="E66" t="n">
+        <v>30</v>
+      </c>
+      <c r="F66" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>Мусин Р.М.</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>44.4</v>
+      </c>
+      <c r="D67" t="n">
+        <v>222</v>
+      </c>
+      <c r="E67" t="n">
+        <v>30</v>
+      </c>
+      <c r="F67" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Наротьев М.А.</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="n">
+        <v>34</v>
+      </c>
+      <c r="D68" t="n">
+        <v>34</v>
+      </c>
+      <c r="E68" t="n">
+        <v>34</v>
+      </c>
+      <c r="F68" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Неустроева С.В.</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
+      </c>
+      <c r="C69" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="D69" t="n">
+        <v>211</v>
+      </c>
+      <c r="E69" t="n">
+        <v>48</v>
+      </c>
+      <c r="F69" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>Нехаев А.В.</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" t="n">
+        <v>50.25</v>
+      </c>
+      <c r="D70" t="n">
+        <v>201</v>
+      </c>
+      <c r="E70" t="n">
+        <v>33</v>
+      </c>
+      <c r="F70" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>Нижневский П.А.</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" t="n">
+        <v>46</v>
+      </c>
+      <c r="D71" t="n">
+        <v>46</v>
+      </c>
+      <c r="E71" t="n">
+        <v>46</v>
+      </c>
+      <c r="F71" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>Новожилов С.В.</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>4</v>
+      </c>
+      <c r="C72" t="n">
+        <v>53</v>
+      </c>
+      <c r="D72" t="n">
+        <v>212</v>
+      </c>
+      <c r="E72" t="n">
+        <v>44</v>
+      </c>
+      <c r="F72" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>Ноздряков М.С</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="n">
+        <v>62</v>
+      </c>
+      <c r="D73" t="n">
+        <v>62</v>
+      </c>
+      <c r="E73" t="n">
+        <v>62</v>
+      </c>
+      <c r="F73" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Носова А.А.</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>3</v>
+      </c>
+      <c r="C74" t="n">
+        <v>66.33333333333333</v>
+      </c>
+      <c r="D74" t="n">
+        <v>199</v>
+      </c>
+      <c r="E74" t="n">
+        <v>51</v>
+      </c>
+      <c r="F74" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Павленко Г.Е.</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="D75" t="n">
+        <v>237</v>
+      </c>
+      <c r="E75" t="n">
+        <v>30</v>
+      </c>
+      <c r="F75" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Першин А.А.</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="D76" t="n">
+        <v>214</v>
+      </c>
+      <c r="E76" t="n">
+        <v>30</v>
+      </c>
+      <c r="F76" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Пилатова А.Е. </t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>4</v>
+      </c>
+      <c r="C77" t="n">
+        <v>51.25</v>
+      </c>
+      <c r="D77" t="n">
+        <v>205</v>
+      </c>
+      <c r="E77" t="n">
+        <v>42</v>
+      </c>
+      <c r="F77" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Ратникова Т.И.</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>4</v>
+      </c>
+      <c r="C78" t="n">
+        <v>51.25</v>
+      </c>
+      <c r="D78" t="n">
+        <v>205</v>
+      </c>
+      <c r="E78" t="n">
+        <v>34</v>
+      </c>
+      <c r="F78" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Савченко А.В.</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="D79" t="n">
+        <v>233</v>
+      </c>
+      <c r="E79" t="n">
+        <v>29</v>
+      </c>
+      <c r="F79" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>Садов К.К.</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>49</v>
+      </c>
+      <c r="D80" t="n">
+        <v>245</v>
+      </c>
+      <c r="E80" t="n">
+        <v>29</v>
+      </c>
+      <c r="F80" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Сажнева О.В.</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>3</v>
+      </c>
+      <c r="C81" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="D81" t="n">
+        <v>205</v>
+      </c>
+      <c r="E81" t="n">
+        <v>57</v>
+      </c>
+      <c r="F81" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Свечников В.В.</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="D82" t="n">
+        <v>243</v>
+      </c>
+      <c r="E82" t="n">
+        <v>25</v>
+      </c>
+      <c r="F82" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Серухин А.В.</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>5</v>
+      </c>
+      <c r="C83" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="D83" t="n">
+        <v>248</v>
+      </c>
+      <c r="E83" t="n">
+        <v>40</v>
+      </c>
+      <c r="F83" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Силаева О.И.</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="D84" t="n">
+        <v>211</v>
+      </c>
+      <c r="E84" t="n">
+        <v>61</v>
+      </c>
+      <c r="F84" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Сироткин А.Н.</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>6</v>
+      </c>
+      <c r="C85" t="n">
+        <v>40.83333333333334</v>
+      </c>
+      <c r="D85" t="n">
+        <v>245</v>
+      </c>
+      <c r="E85" t="n">
+        <v>30</v>
+      </c>
+      <c r="F85" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Скрябин С.Н.</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>5</v>
+      </c>
+      <c r="C86" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="D86" t="n">
+        <v>233</v>
+      </c>
+      <c r="E86" t="n">
+        <v>32</v>
+      </c>
+      <c r="F86" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Смирнова О.В.</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>42</v>
+      </c>
+      <c r="D87" t="n">
+        <v>210</v>
+      </c>
+      <c r="E87" t="n">
+        <v>20</v>
+      </c>
+      <c r="F87" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Солодовникова Н.В.</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>3</v>
+      </c>
+      <c r="C88" t="n">
+        <v>55.66666666666666</v>
+      </c>
+      <c r="D88" t="n">
+        <v>167</v>
+      </c>
+      <c r="E88" t="n">
+        <v>49</v>
+      </c>
+      <c r="F88" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Солтан Д. С.</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>4</v>
+      </c>
+      <c r="C89" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="D89" t="n">
+        <v>194</v>
+      </c>
+      <c r="E89" t="n">
+        <v>41</v>
+      </c>
+      <c r="F89" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Столярова И.В.</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>60.33333333333334</v>
+      </c>
+      <c r="D90" t="n">
+        <v>181</v>
+      </c>
+      <c r="E90" t="n">
+        <v>54</v>
+      </c>
+      <c r="F90" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Таковникова Н.А.</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>2</v>
+      </c>
+      <c r="C91" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="D91" t="n">
+        <v>143</v>
+      </c>
+      <c r="E91" t="n">
+        <v>67</v>
+      </c>
+      <c r="F91" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>Тарасова Ю.П.</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" t="n">
+        <v>67</v>
+      </c>
+      <c r="D92" t="n">
+        <v>201</v>
+      </c>
+      <c r="E92" t="n">
+        <v>52</v>
+      </c>
+      <c r="F92" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Теленкова В.А.</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2</v>
+      </c>
+      <c r="C93" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="D93" t="n">
+        <v>213</v>
+      </c>
+      <c r="E93" t="n">
+        <v>100</v>
+      </c>
+      <c r="F93" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Тимонин А.В.</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="D94" t="n">
+        <v>253</v>
+      </c>
+      <c r="E94" t="n">
+        <v>41</v>
+      </c>
+      <c r="F94" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Тихомирова Е.Е.</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>3</v>
+      </c>
+      <c r="C95" t="n">
+        <v>70.66666666666667</v>
+      </c>
+      <c r="D95" t="n">
+        <v>212</v>
+      </c>
+      <c r="E95" t="n">
+        <v>52</v>
+      </c>
+      <c r="F95" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Тришкина Е.В.</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>2</v>
+      </c>
+      <c r="C96" t="n">
+        <v>65</v>
+      </c>
+      <c r="D96" t="n">
+        <v>130</v>
+      </c>
+      <c r="E96" t="n">
+        <v>62</v>
+      </c>
+      <c r="F96" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Тушинок С.Н.</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>3</v>
+      </c>
+      <c r="C97" t="n">
+        <v>57.33333333333334</v>
+      </c>
+      <c r="D97" t="n">
+        <v>172</v>
+      </c>
+      <c r="E97" t="n">
+        <v>49</v>
+      </c>
+      <c r="F97" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Удовенко М.С.</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>4</v>
+      </c>
+      <c r="C98" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="D98" t="n">
+        <v>173</v>
+      </c>
+      <c r="E98" t="n">
+        <v>28</v>
+      </c>
+      <c r="F98" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Уткин Н.С.</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>5</v>
+      </c>
+      <c r="C99" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="D99" t="n">
+        <v>228</v>
+      </c>
+      <c r="E99" t="n">
+        <v>30</v>
+      </c>
+      <c r="F99" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Филиппов В.М.</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>3</v>
+      </c>
+      <c r="C100" t="n">
+        <v>49.33333333333334</v>
+      </c>
+      <c r="D100" t="n">
+        <v>148</v>
+      </c>
+      <c r="E100" t="n">
+        <v>36</v>
+      </c>
+      <c r="F100" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Фокина Е.А.</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>4</v>
+      </c>
+      <c r="C101" t="n">
+        <v>49.25</v>
+      </c>
+      <c r="D101" t="n">
+        <v>197</v>
+      </c>
+      <c r="E101" t="n">
+        <v>45</v>
+      </c>
+      <c r="F101" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Хализев В.И.</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" t="n">
+        <v>34</v>
+      </c>
+      <c r="D102" t="n">
+        <v>34</v>
+      </c>
+      <c r="E102" t="n">
+        <v>34</v>
+      </c>
+      <c r="F102" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Ходорко В.Э.</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>4</v>
+      </c>
+      <c r="C103" t="n">
+        <v>47</v>
+      </c>
+      <c r="D103" t="n">
+        <v>188</v>
+      </c>
+      <c r="E103" t="n">
+        <v>39</v>
+      </c>
+      <c r="F103" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Ходченкова М.Н.</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>3</v>
+      </c>
+      <c r="C104" t="n">
+        <v>62.33333333333334</v>
+      </c>
+      <c r="D104" t="n">
+        <v>187</v>
+      </c>
+      <c r="E104" t="n">
+        <v>39</v>
+      </c>
+      <c r="F104" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Христофорова О.С.</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>3</v>
+      </c>
+      <c r="C105" t="n">
+        <v>53.66666666666666</v>
+      </c>
+      <c r="D105" t="n">
+        <v>161</v>
+      </c>
+      <c r="E105" t="n">
+        <v>46</v>
+      </c>
+      <c r="F105" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Цыбаков С.Ю</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>6</v>
+      </c>
+      <c r="C106" t="n">
+        <v>43.33333333333334</v>
+      </c>
+      <c r="D106" t="n">
+        <v>260</v>
+      </c>
+      <c r="E106" t="n">
+        <v>34</v>
+      </c>
+      <c r="F106" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Чернявская В.А.</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>4</v>
+      </c>
+      <c r="C107" t="n">
+        <v>51.25</v>
+      </c>
+      <c r="D107" t="n">
+        <v>205</v>
+      </c>
+      <c r="E107" t="n">
+        <v>25</v>
+      </c>
+      <c r="F107" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Шварева М.В.</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" t="n">
+        <v>50</v>
+      </c>
+      <c r="D108" t="n">
+        <v>50</v>
+      </c>
+      <c r="E108" t="n">
+        <v>50</v>
+      </c>
+      <c r="F108" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>Шейман И.Г.</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>6</v>
+      </c>
+      <c r="C109" t="n">
+        <v>43.83333333333334</v>
+      </c>
+      <c r="D109" t="n">
+        <v>263</v>
+      </c>
+      <c r="E109" t="n">
+        <v>30</v>
+      </c>
+      <c r="F109" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Шипунов А.В.</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="D110" t="n">
+        <v>233</v>
+      </c>
+      <c r="E110" t="n">
+        <v>33</v>
+      </c>
+      <c r="F110" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Шувалова Т.А.</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>5</v>
+      </c>
+      <c r="C111" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="D111" t="n">
+        <v>211</v>
+      </c>
+      <c r="E111" t="n">
+        <v>20</v>
+      </c>
+      <c r="F111" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
           <t>Шуйкова С.М.</t>
         </is>
       </c>
-      <c r="B63" t="n">
+      <c r="B112" t="n">
         <v>4</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C112" t="n">
         <v>53.25</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D112" t="n">
         <v>213</v>
       </c>
-      <c r="E63" t="n">
+      <c r="E112" t="n">
         <v>44</v>
       </c>
-      <c r="F63" t="n">
+      <c r="F112" t="n">
         <v>65</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Щедрин М.А.</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>5</v>
+      </c>
+      <c r="C113" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="D113" t="n">
+        <v>232</v>
+      </c>
+      <c r="E113" t="n">
+        <v>34</v>
+      </c>
+      <c r="F113" t="n">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs and add distribution in html
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,966 +511,966 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Аниськина Е.А.</t>
+          <t>Аггеев Д.А.</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>52</v>
+        <v>50.6</v>
       </c>
       <c r="D4" t="n">
-        <v>156</v>
+        <v>253</v>
       </c>
       <c r="E4" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F4" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Афанасьева Н.В.</t>
+          <t>Акимов В.И.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>42.33333333333334</v>
+        <v>43.33333333333334</v>
       </c>
       <c r="D5" t="n">
-        <v>127</v>
+        <v>260</v>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Белоусова Е,В.</t>
+          <t>Акульшин А.П.</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>61.5</v>
+        <v>37.6</v>
       </c>
       <c r="D6" t="n">
-        <v>123</v>
+        <v>188</v>
       </c>
       <c r="E6" t="n">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Болвачева И. А.</t>
+          <t>Алексеев А.Г.</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>49.25</v>
+        <v>50</v>
       </c>
       <c r="D7" t="n">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Бубнова Е.В.</t>
+          <t>Андрианов С.Д,</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>71</v>
+        <v>51.2</v>
       </c>
       <c r="D8" t="n">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="E8" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F8" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Горохова Е.Н.</t>
+          <t>Аниськина Е.А.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>48</v>
+        <v>49.25</v>
       </c>
       <c r="D9" t="n">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="E9" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Гусева Н.И.</t>
+          <t>Арзамасцев В.В.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D10" t="n">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F10" t="n">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Жукова Г.Б.</t>
+          <t>Афанасьева Н.В.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>52.33333333333334</v>
+        <v>48.25</v>
       </c>
       <c r="D11" t="n">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="E11" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F11" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Захарова К.Г.</t>
+          <t>Бабенков А. А.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>73</v>
+        <v>41.83333333333334</v>
       </c>
       <c r="D12" t="n">
-        <v>146</v>
+        <v>251</v>
       </c>
       <c r="E12" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Исаева Э.Е.</t>
+          <t>Белоусова Е,В.</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>52.33333333333334</v>
+        <v>60.66666666666666</v>
       </c>
       <c r="D13" t="n">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="E13" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F13" t="n">
-        <v>63</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Карева Т.Ю.</t>
+          <t>Билжа С.Й</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>67.5</v>
+        <v>41</v>
       </c>
       <c r="D14" t="n">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="E14" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="F14" t="n">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Киселева Н.В.</t>
+          <t>Бодров О.В.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>98</v>
+        <v>40.83333333333334</v>
       </c>
       <c r="D15" t="n">
-        <v>98</v>
+        <v>245</v>
       </c>
       <c r="E15" t="n">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="F15" t="n">
-        <v>98</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Ковалева Ю.Г.</t>
+          <t>Болвачева И. А.</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>81.5</v>
+        <v>49.25</v>
       </c>
       <c r="D16" t="n">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="E16" t="n">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="F16" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Козлова Е. В.</t>
+          <t>Болотов Г.Е.</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D17" t="n">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E17" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F17" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Колесникова Е,И.</t>
+          <t>Борисов А.Ю.</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>69</v>
+        <v>42.4</v>
       </c>
       <c r="D18" t="n">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="E18" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F18" t="n">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Кондратенко А.Н.</t>
+          <t>Боталов А.М.</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>66.5</v>
+        <v>40.4</v>
       </c>
       <c r="D19" t="n">
-        <v>133</v>
+        <v>202</v>
       </c>
       <c r="E19" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="F19" t="n">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Кузнецов Е.Б.</t>
+          <t>Бубнова Е.В.</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D20" t="n">
-        <v>156</v>
+        <v>213</v>
       </c>
       <c r="E20" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F20" t="n">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Куклина Ф.Н.</t>
+          <t>Будников А.В.</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>211</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+      <c r="F21" t="n">
         <v>52</v>
-      </c>
-      <c r="D21" t="n">
-        <v>156</v>
-      </c>
-      <c r="E21" t="n">
-        <v>38</v>
-      </c>
-      <c r="F21" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Курочкина И.В.</t>
+          <t>Бушуев А.А.</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>61.66666666666666</v>
+        <v>49.5</v>
       </c>
       <c r="D22" t="n">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="E22" t="n">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="F22" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Лобова Е.В.</t>
+          <t>Быков Е.А.</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>70.5</v>
+        <v>49.2</v>
       </c>
       <c r="D23" t="n">
-        <v>141</v>
+        <v>246</v>
       </c>
       <c r="E23" t="n">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="F23" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Макарова А.С.</t>
+          <t>Викторов В.В.</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>104</v>
+        <v>58.25</v>
       </c>
       <c r="D24" t="n">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="E24" t="n">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="F24" t="n">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Марухина Н.А.</t>
+          <t>Вихров Р.Т.</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D25" t="n">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="E25" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F25" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Минкина Е.К.</t>
+          <t>Воробьёв С.В.</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>71</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="D26" t="n">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="E26" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Миронова Л.В.</t>
+          <t>Гавриленко О.В.</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>59.33333333333334</v>
+        <v>50.25</v>
       </c>
       <c r="D27" t="n">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="E27" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F27" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Неустроева С.В.</t>
+          <t>Герасименко А.Т.</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>64</v>
+        <v>39.83333333333334</v>
       </c>
       <c r="D28" t="n">
-        <v>192</v>
+        <v>239</v>
       </c>
       <c r="E28" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Нехаев А.В.</t>
+          <t>Горностаев И.Б.</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>69.33333333333333</v>
+        <v>44.75</v>
       </c>
       <c r="D29" t="n">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="E29" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F29" t="n">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Новожилов С.В.</t>
+          <t>Горохова Е.Н.</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D30" t="n">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="E30" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F30" t="n">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Носова А.А.</t>
+          <t>Гусева Н.И.</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>53.33333333333334</v>
+        <v>41.6</v>
       </c>
       <c r="D31" t="n">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="E31" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F31" t="n">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Пилатова А.Е. </t>
+          <t>Демидов А.С.</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D32" t="n">
-        <v>129</v>
+        <v>232</v>
       </c>
       <c r="E32" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F32" t="n">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Ратникова Т.И.</t>
+          <t>Дядищев С.В.</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>48.75</v>
+        <v>49.5</v>
       </c>
       <c r="D33" t="n">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E33" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F33" t="n">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Сажнева О.В.</t>
+          <t>Ефремов П.С,</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>68.33333333333333</v>
+        <v>45.6</v>
       </c>
       <c r="D34" t="n">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="E34" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F34" t="n">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Силаева О.И.</t>
+          <t>Жукова Г.Б.</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
+        <v>53.25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>213</v>
+      </c>
+      <c r="E35" t="n">
+        <v>45</v>
+      </c>
+      <c r="F35" t="n">
         <v>60</v>
-      </c>
-      <c r="D35" t="n">
-        <v>180</v>
-      </c>
-      <c r="E35" t="n">
-        <v>52</v>
-      </c>
-      <c r="F35" t="n">
-        <v>68</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Смирнова О.В.</t>
+          <t>Захаров Д.И.</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>71.5</v>
+        <v>44.33333333333334</v>
       </c>
       <c r="D36" t="n">
-        <v>143</v>
+        <v>266</v>
       </c>
       <c r="E36" t="n">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F36" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Солодовникова Н.В.</t>
+          <t>Захарова К.Г.</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>65.5</v>
+        <v>73</v>
       </c>
       <c r="D37" t="n">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E37" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F37" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Столярова И.В.</t>
+          <t>Зиновьев С.В.</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>53.66666666666666</v>
+        <v>50.2</v>
       </c>
       <c r="D38" t="n">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="E38" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F38" t="n">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Таковникова Н.А.</t>
+          <t>Инкин Г.А.</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C39" t="n">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="D39" t="n">
-        <v>138</v>
+        <v>215</v>
       </c>
       <c r="E39" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="F39" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Тарасова Ю.П.</t>
+          <t>Исаев М.М.</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>48</v>
+        <v>42.25</v>
       </c>
       <c r="D40" t="n">
-        <v>96</v>
+        <v>169</v>
       </c>
       <c r="E40" t="n">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F40" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Теленкова В.А.</t>
+          <t>Исаева Э.Е.</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>68</v>
+        <v>51.5</v>
       </c>
       <c r="D41" t="n">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="E41" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F41" t="n">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Тихомирова Е.Е.</t>
+          <t>Карева Т.Ю.</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>60.66666666666666</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="D42" t="n">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E42" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F42" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Тришкина Е.В.</t>
+          <t>Киселева Н.В.</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D43" t="n">
-        <v>153</v>
+        <v>98</v>
       </c>
       <c r="E43" t="n">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="F43" t="n">
-        <v>56</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Тушинок С.Н.</t>
+          <t>Кобзев Д.В.</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>69</v>
+        <v>68.66666666666667</v>
       </c>
       <c r="D44" t="n">
-        <v>138</v>
+        <v>206</v>
       </c>
       <c r="E44" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="F44" t="n">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Удовенко М.С.</t>
+          <t>Ковалева Ю.Г.</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>72.5</v>
+        <v>70.66666666666667</v>
       </c>
       <c r="D45" t="n">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="E45" t="n">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F45" t="n">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Фокина Е.А.</t>
+          <t>Коваленко А.В.</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>51.33333333333334</v>
+        <v>49</v>
       </c>
       <c r="D46" t="n">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="E46" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F46" t="n">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Ходченкова М.Н.</t>
+          <t>Козлова Е. В.</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>71.5</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="D47" t="n">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="E47" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F47" t="n">
         <v>76</v>
@@ -1479,111 +1479,1585 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Христофорова О.С.</t>
+          <t>Колесникова Е,И.</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" t="n">
-        <v>66</v>
+        <v>64.33333333333333</v>
       </c>
       <c r="D48" t="n">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="E48" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F48" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Чернявская В.А.</t>
+          <t>Колобков К.М</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C49" t="n">
-        <v>72</v>
+        <v>46.6</v>
       </c>
       <c r="D49" t="n">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="E49" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F49" t="n">
-        <v>101</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Шварева М.В.</t>
+          <t>Кольцов М.Ю.</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>61.5</v>
+        <v>50.6</v>
       </c>
       <c r="D50" t="n">
-        <v>123</v>
+        <v>253</v>
       </c>
       <c r="E50" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F50" t="n">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Шувалова Т.А.</t>
+          <t>Кондратенко А.Н.</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>39.5</v>
+        <v>66.5</v>
       </c>
       <c r="D51" t="n">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="E51" t="n">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="F51" t="n">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
+          <t>Корнеев К.В.</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="D52" t="n">
+        <v>229</v>
+      </c>
+      <c r="E52" t="n">
+        <v>29</v>
+      </c>
+      <c r="F52" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>Костин В.Ю.</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="D53" t="n">
+        <v>223</v>
+      </c>
+      <c r="E53" t="n">
+        <v>36</v>
+      </c>
+      <c r="F53" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Костюков Н.В.</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>6</v>
+      </c>
+      <c r="C54" t="n">
+        <v>41.66666666666666</v>
+      </c>
+      <c r="D54" t="n">
+        <v>250</v>
+      </c>
+      <c r="E54" t="n">
+        <v>30</v>
+      </c>
+      <c r="F54" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Кузнецов А.В. </t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="D55" t="n">
+        <v>263</v>
+      </c>
+      <c r="E55" t="n">
+        <v>44</v>
+      </c>
+      <c r="F55" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Кузнецов Е.Б.</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" t="n">
+        <v>52.25</v>
+      </c>
+      <c r="D56" t="n">
+        <v>209</v>
+      </c>
+      <c r="E56" t="n">
+        <v>38</v>
+      </c>
+      <c r="F56" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>Кузьмичев В.К.</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>37</v>
+      </c>
+      <c r="D57" t="n">
+        <v>74</v>
+      </c>
+      <c r="E57" t="n">
+        <v>34</v>
+      </c>
+      <c r="F57" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Куклина Ф.Н.</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" t="n">
+        <v>52</v>
+      </c>
+      <c r="D58" t="n">
+        <v>156</v>
+      </c>
+      <c r="E58" t="n">
+        <v>38</v>
+      </c>
+      <c r="F58" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>Курочкина И.В.</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>3</v>
+      </c>
+      <c r="C59" t="n">
+        <v>61.66666666666666</v>
+      </c>
+      <c r="D59" t="n">
+        <v>185</v>
+      </c>
+      <c r="E59" t="n">
+        <v>55</v>
+      </c>
+      <c r="F59" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Лазутин Д.В.</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>6</v>
+      </c>
+      <c r="C60" t="n">
+        <v>43.83333333333334</v>
+      </c>
+      <c r="D60" t="n">
+        <v>263</v>
+      </c>
+      <c r="E60" t="n">
+        <v>30</v>
+      </c>
+      <c r="F60" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>Лобова Е.В.</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" t="n">
+        <v>65</v>
+      </c>
+      <c r="D61" t="n">
+        <v>195</v>
+      </c>
+      <c r="E61" t="n">
+        <v>54</v>
+      </c>
+      <c r="F61" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Лыков К.А.</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>6</v>
+      </c>
+      <c r="C62" t="n">
+        <v>41.83333333333334</v>
+      </c>
+      <c r="D62" t="n">
+        <v>251</v>
+      </c>
+      <c r="E62" t="n">
+        <v>30</v>
+      </c>
+      <c r="F62" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>Мазеин А.П.</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="n">
+        <v>44</v>
+      </c>
+      <c r="D63" t="n">
+        <v>264</v>
+      </c>
+      <c r="E63" t="n">
+        <v>37</v>
+      </c>
+      <c r="F63" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>Макарова А.С.</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>104</v>
+      </c>
+      <c r="D64" t="n">
+        <v>208</v>
+      </c>
+      <c r="E64" t="n">
+        <v>100</v>
+      </c>
+      <c r="F64" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>Марухина Н.А.</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>53</v>
+      </c>
+      <c r="D65" t="n">
+        <v>159</v>
+      </c>
+      <c r="E65" t="n">
+        <v>41</v>
+      </c>
+      <c r="F65" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Медведев П.С.</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>4</v>
+      </c>
+      <c r="C66" t="n">
+        <v>49.75</v>
+      </c>
+      <c r="D66" t="n">
+        <v>199</v>
+      </c>
+      <c r="E66" t="n">
+        <v>44</v>
+      </c>
+      <c r="F66" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>Минкина Е.К.</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C67" t="n">
+        <v>71</v>
+      </c>
+      <c r="D67" t="n">
+        <v>213</v>
+      </c>
+      <c r="E67" t="n">
+        <v>62</v>
+      </c>
+      <c r="F67" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Миронова Л.В.</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="n">
+        <v>59.33333333333334</v>
+      </c>
+      <c r="D68" t="n">
+        <v>178</v>
+      </c>
+      <c r="E68" t="n">
+        <v>40</v>
+      </c>
+      <c r="F68" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Мурзак Д.Г.</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>4</v>
+      </c>
+      <c r="C69" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="D69" t="n">
+        <v>214</v>
+      </c>
+      <c r="E69" t="n">
+        <v>48</v>
+      </c>
+      <c r="F69" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>Мусин Р.М.</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="D70" t="n">
+        <v>214</v>
+      </c>
+      <c r="E70" t="n">
+        <v>48</v>
+      </c>
+      <c r="F70" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>Наротьев М.А.</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>3</v>
+      </c>
+      <c r="C71" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="D71" t="n">
+        <v>133</v>
+      </c>
+      <c r="E71" t="n">
+        <v>33</v>
+      </c>
+      <c r="F71" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>Неустроева С.В.</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C72" t="n">
+        <v>64</v>
+      </c>
+      <c r="D72" t="n">
+        <v>192</v>
+      </c>
+      <c r="E72" t="n">
+        <v>59</v>
+      </c>
+      <c r="F72" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>Нехаев А.В.</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3</v>
+      </c>
+      <c r="C73" t="n">
+        <v>69.33333333333333</v>
+      </c>
+      <c r="D73" t="n">
+        <v>208</v>
+      </c>
+      <c r="E73" t="n">
+        <v>58</v>
+      </c>
+      <c r="F73" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Нижневский П.А.</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>3</v>
+      </c>
+      <c r="C74" t="n">
+        <v>40</v>
+      </c>
+      <c r="D74" t="n">
+        <v>120</v>
+      </c>
+      <c r="E74" t="n">
+        <v>34</v>
+      </c>
+      <c r="F74" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Новожилов С.В.</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="n">
+        <v>67.66666666666667</v>
+      </c>
+      <c r="D75" t="n">
+        <v>203</v>
+      </c>
+      <c r="E75" t="n">
+        <v>46</v>
+      </c>
+      <c r="F75" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Ноздряков М.С</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2</v>
+      </c>
+      <c r="C76" t="n">
+        <v>70</v>
+      </c>
+      <c r="D76" t="n">
+        <v>140</v>
+      </c>
+      <c r="E76" t="n">
+        <v>61</v>
+      </c>
+      <c r="F76" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Носова А.А.</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>4</v>
+      </c>
+      <c r="C77" t="n">
+        <v>52.75</v>
+      </c>
+      <c r="D77" t="n">
+        <v>211</v>
+      </c>
+      <c r="E77" t="n">
+        <v>40</v>
+      </c>
+      <c r="F77" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Павленко Г.Е.</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="D78" t="n">
+        <v>239</v>
+      </c>
+      <c r="E78" t="n">
+        <v>34</v>
+      </c>
+      <c r="F78" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Першин А.А.</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>4</v>
+      </c>
+      <c r="C79" t="n">
+        <v>47</v>
+      </c>
+      <c r="D79" t="n">
+        <v>188</v>
+      </c>
+      <c r="E79" t="n">
+        <v>32</v>
+      </c>
+      <c r="F79" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Пилатова А.Е. </t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="D80" t="n">
+        <v>195</v>
+      </c>
+      <c r="E80" t="n">
+        <v>28</v>
+      </c>
+      <c r="F80" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Ратникова Т.И.</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>4</v>
+      </c>
+      <c r="C81" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="D81" t="n">
+        <v>195</v>
+      </c>
+      <c r="E81" t="n">
+        <v>34</v>
+      </c>
+      <c r="F81" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Савченко А.В.</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="D82" t="n">
+        <v>251</v>
+      </c>
+      <c r="E82" t="n">
+        <v>41</v>
+      </c>
+      <c r="F82" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Садов К.К.</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>4</v>
+      </c>
+      <c r="C83" t="n">
+        <v>55.75</v>
+      </c>
+      <c r="D83" t="n">
+        <v>223</v>
+      </c>
+      <c r="E83" t="n">
+        <v>36</v>
+      </c>
+      <c r="F83" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Сажнева О.В.</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="D84" t="n">
+        <v>205</v>
+      </c>
+      <c r="E84" t="n">
+        <v>49</v>
+      </c>
+      <c r="F84" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Свечников В.В.</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>4</v>
+      </c>
+      <c r="C85" t="n">
+        <v>55.75</v>
+      </c>
+      <c r="D85" t="n">
+        <v>223</v>
+      </c>
+      <c r="E85" t="n">
+        <v>47</v>
+      </c>
+      <c r="F85" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Серухин А.В.</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>6</v>
+      </c>
+      <c r="C86" t="n">
+        <v>43.66666666666666</v>
+      </c>
+      <c r="D86" t="n">
+        <v>262</v>
+      </c>
+      <c r="E86" t="n">
+        <v>30</v>
+      </c>
+      <c r="F86" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Силаева О.И.</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" t="n">
+        <v>60</v>
+      </c>
+      <c r="D87" t="n">
+        <v>180</v>
+      </c>
+      <c r="E87" t="n">
+        <v>52</v>
+      </c>
+      <c r="F87" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Синяков А.В.</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>2</v>
+      </c>
+      <c r="C88" t="n">
+        <v>37</v>
+      </c>
+      <c r="D88" t="n">
+        <v>74</v>
+      </c>
+      <c r="E88" t="n">
+        <v>34</v>
+      </c>
+      <c r="F88" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Сироткин А.Н.</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" t="n">
+        <v>50</v>
+      </c>
+      <c r="D89" t="n">
+        <v>150</v>
+      </c>
+      <c r="E89" t="n">
+        <v>39</v>
+      </c>
+      <c r="F89" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Скрябин С.Н.</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>51.66666666666666</v>
+      </c>
+      <c r="D90" t="n">
+        <v>155</v>
+      </c>
+      <c r="E90" t="n">
+        <v>37</v>
+      </c>
+      <c r="F90" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Смирнова О.В.</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" t="n">
+        <v>65.66666666666667</v>
+      </c>
+      <c r="D91" t="n">
+        <v>197</v>
+      </c>
+      <c r="E91" t="n">
+        <v>53</v>
+      </c>
+      <c r="F91" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>Солодовникова Н.В.</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>2</v>
+      </c>
+      <c r="C92" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="D92" t="n">
+        <v>131</v>
+      </c>
+      <c r="E92" t="n">
+        <v>61</v>
+      </c>
+      <c r="F92" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Солтан Д. С.</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="D93" t="n">
+        <v>239</v>
+      </c>
+      <c r="E93" t="n">
+        <v>36</v>
+      </c>
+      <c r="F93" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Столярова И.В.</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" t="n">
+        <v>53.66666666666666</v>
+      </c>
+      <c r="D94" t="n">
+        <v>161</v>
+      </c>
+      <c r="E94" t="n">
+        <v>49</v>
+      </c>
+      <c r="F94" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Таковникова Н.А.</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>3</v>
+      </c>
+      <c r="C95" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="D95" t="n">
+        <v>211</v>
+      </c>
+      <c r="E95" t="n">
+        <v>61</v>
+      </c>
+      <c r="F95" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Тарасова Ю.П.</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>3</v>
+      </c>
+      <c r="C96" t="n">
+        <v>56.33333333333334</v>
+      </c>
+      <c r="D96" t="n">
+        <v>169</v>
+      </c>
+      <c r="E96" t="n">
+        <v>48</v>
+      </c>
+      <c r="F96" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Теленкова В.А.</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>3</v>
+      </c>
+      <c r="C97" t="n">
+        <v>62</v>
+      </c>
+      <c r="D97" t="n">
+        <v>186</v>
+      </c>
+      <c r="E97" t="n">
+        <v>45</v>
+      </c>
+      <c r="F97" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Тимонин А.В.</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>6</v>
+      </c>
+      <c r="C98" t="n">
+        <v>42</v>
+      </c>
+      <c r="D98" t="n">
+        <v>252</v>
+      </c>
+      <c r="E98" t="n">
+        <v>31</v>
+      </c>
+      <c r="F98" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Тихомирова Е.Е.</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>3</v>
+      </c>
+      <c r="C99" t="n">
+        <v>60.66666666666666</v>
+      </c>
+      <c r="D99" t="n">
+        <v>182</v>
+      </c>
+      <c r="E99" t="n">
+        <v>48</v>
+      </c>
+      <c r="F99" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Тришкина Е.В.</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>4</v>
+      </c>
+      <c r="C100" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="D100" t="n">
+        <v>206</v>
+      </c>
+      <c r="E100" t="n">
+        <v>47</v>
+      </c>
+      <c r="F100" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Тушинок С.Н.</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>3</v>
+      </c>
+      <c r="C101" t="n">
+        <v>66.66666666666667</v>
+      </c>
+      <c r="D101" t="n">
+        <v>200</v>
+      </c>
+      <c r="E101" t="n">
+        <v>62</v>
+      </c>
+      <c r="F101" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Удовенко М.С.</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C102" t="n">
+        <v>64.66666666666667</v>
+      </c>
+      <c r="D102" t="n">
+        <v>194</v>
+      </c>
+      <c r="E102" t="n">
+        <v>49</v>
+      </c>
+      <c r="F102" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Уткин Н.С.</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>5</v>
+      </c>
+      <c r="C103" t="n">
+        <v>53</v>
+      </c>
+      <c r="D103" t="n">
+        <v>265</v>
+      </c>
+      <c r="E103" t="n">
+        <v>41</v>
+      </c>
+      <c r="F103" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Филиппов В.М.</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>5</v>
+      </c>
+      <c r="C104" t="n">
+        <v>46</v>
+      </c>
+      <c r="D104" t="n">
+        <v>230</v>
+      </c>
+      <c r="E104" t="n">
+        <v>37</v>
+      </c>
+      <c r="F104" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Фокина Е.А.</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>4</v>
+      </c>
+      <c r="C105" t="n">
+        <v>49</v>
+      </c>
+      <c r="D105" t="n">
+        <v>196</v>
+      </c>
+      <c r="E105" t="n">
+        <v>32</v>
+      </c>
+      <c r="F105" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Фролов К.В.</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" t="n">
+        <v>79</v>
+      </c>
+      <c r="D106" t="n">
+        <v>79</v>
+      </c>
+      <c r="E106" t="n">
+        <v>79</v>
+      </c>
+      <c r="F106" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Хализев В.И.</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>3</v>
+      </c>
+      <c r="C107" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="D107" t="n">
+        <v>133</v>
+      </c>
+      <c r="E107" t="n">
+        <v>33</v>
+      </c>
+      <c r="F107" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Ходорко В.Э.</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>5</v>
+      </c>
+      <c r="C108" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="D108" t="n">
+        <v>213</v>
+      </c>
+      <c r="E108" t="n">
+        <v>31</v>
+      </c>
+      <c r="F108" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>Ходченкова М.Н.</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>3</v>
+      </c>
+      <c r="C109" t="n">
+        <v>69.33333333333333</v>
+      </c>
+      <c r="D109" t="n">
+        <v>208</v>
+      </c>
+      <c r="E109" t="n">
+        <v>65</v>
+      </c>
+      <c r="F109" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Христофорова О.С.</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>3</v>
+      </c>
+      <c r="C110" t="n">
+        <v>61.33333333333334</v>
+      </c>
+      <c r="D110" t="n">
+        <v>184</v>
+      </c>
+      <c r="E110" t="n">
+        <v>52</v>
+      </c>
+      <c r="F110" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Цыбаков С.Ю</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>5</v>
+      </c>
+      <c r="C111" t="n">
+        <v>43.8</v>
+      </c>
+      <c r="D111" t="n">
+        <v>219</v>
+      </c>
+      <c r="E111" t="n">
+        <v>32</v>
+      </c>
+      <c r="F111" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Чернявская В.А.</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>3</v>
+      </c>
+      <c r="C112" t="n">
+        <v>70</v>
+      </c>
+      <c r="D112" t="n">
+        <v>210</v>
+      </c>
+      <c r="E112" t="n">
+        <v>43</v>
+      </c>
+      <c r="F112" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Шарфутов А.В.</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>2</v>
+      </c>
+      <c r="C113" t="n">
+        <v>40</v>
+      </c>
+      <c r="D113" t="n">
+        <v>80</v>
+      </c>
+      <c r="E113" t="n">
+        <v>40</v>
+      </c>
+      <c r="F113" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>Шварева М.В.</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>2</v>
+      </c>
+      <c r="C114" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>123</v>
+      </c>
+      <c r="E114" t="n">
+        <v>50</v>
+      </c>
+      <c r="F114" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Шейман И.Г.</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>6</v>
+      </c>
+      <c r="C115" t="n">
+        <v>40.83333333333334</v>
+      </c>
+      <c r="D115" t="n">
+        <v>245</v>
+      </c>
+      <c r="E115" t="n">
+        <v>30</v>
+      </c>
+      <c r="F115" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>Шипунов А.В.</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>5</v>
+      </c>
+      <c r="C116" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="D116" t="n">
+        <v>258</v>
+      </c>
+      <c r="E116" t="n">
+        <v>37</v>
+      </c>
+      <c r="F116" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Шувалова Т.А.</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>5</v>
+      </c>
+      <c r="C117" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="D117" t="n">
+        <v>213</v>
+      </c>
+      <c r="E117" t="n">
+        <v>25</v>
+      </c>
+      <c r="F117" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
           <t>Шуйкова С.М.</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>2</v>
-      </c>
-      <c r="C52" t="n">
-        <v>69.5</v>
-      </c>
-      <c r="D52" t="n">
-        <v>139</v>
-      </c>
-      <c r="E52" t="n">
-        <v>65</v>
-      </c>
-      <c r="F52" t="n">
+      <c r="B118" t="n">
+        <v>3</v>
+      </c>
+      <c r="C118" t="n">
+        <v>64.33333333333333</v>
+      </c>
+      <c r="D118" t="n">
+        <v>193</v>
+      </c>
+      <c r="E118" t="n">
+        <v>54</v>
+      </c>
+      <c r="F118" t="n">
         <v>74</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>Щедрин М.А.</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>5</v>
+      </c>
+      <c r="C119" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="D119" t="n">
+        <v>263</v>
+      </c>
+      <c r="E119" t="n">
+        <v>41</v>
+      </c>
+      <c r="F119" t="n">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug. when no requests in some date
</commit_message>
<xml_diff>
--- a/stat.xlsx
+++ b/stat.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,966 +511,966 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Аниськина Е.А.</t>
+          <t>Аггеев Д.А.</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>49.25</v>
+        <v>51</v>
       </c>
       <c r="D4" t="n">
-        <v>197</v>
+        <v>255</v>
       </c>
       <c r="E4" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F4" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Афанасьева Н.В.</t>
+          <t>Акимов В.И.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>48.25</v>
+        <v>46</v>
       </c>
       <c r="D5" t="n">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F5" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Белоусова Е,В.</t>
+          <t>Акульшин А.П.</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>60.66666666666666</v>
+        <v>46.4</v>
       </c>
       <c r="D6" t="n">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="E6" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Болвачева И. А.</t>
+          <t>Алексеев А.Г.</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>49.25</v>
+        <v>50</v>
       </c>
       <c r="D7" t="n">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Бубнова Е.В.</t>
+          <t>Андрианов С.Д,</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>71</v>
+        <v>51.2</v>
       </c>
       <c r="D8" t="n">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="E8" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F8" t="n">
-        <v>110</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Горохова Е.Н.</t>
+          <t>Аниськина Е.А.</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>49.25</v>
       </c>
       <c r="D9" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E9" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Гусева Н.И.</t>
+          <t>Арзамасцев В.В.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>41.6</v>
+        <v>70</v>
       </c>
       <c r="D10" t="n">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F10" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Жукова Г.Б.</t>
+          <t>Афанасьева Н.В.</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>53.25</v>
+        <v>48.25</v>
       </c>
       <c r="D11" t="n">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="E11" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F11" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Захарова К.Г.</t>
+          <t>Бабенков А. А.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>73</v>
+        <v>43.5</v>
       </c>
       <c r="D12" t="n">
-        <v>146</v>
+        <v>261</v>
       </c>
       <c r="E12" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Исаева Э.Е.</t>
+          <t>Белоусова Е,В.</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>51.5</v>
+        <v>60.66666666666666</v>
       </c>
       <c r="D13" t="n">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="E13" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F13" t="n">
-        <v>63</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Карева Т.Ю.</t>
+          <t>Билжа С.Й</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>58.66666666666666</v>
+        <v>47</v>
       </c>
       <c r="D14" t="n">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E14" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F14" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Киселева Н.В.</t>
+          <t>Бодров О.В.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>98</v>
+        <v>40.5</v>
       </c>
       <c r="D15" t="n">
-        <v>98</v>
+        <v>243</v>
       </c>
       <c r="E15" t="n">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="F15" t="n">
-        <v>98</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Ковалева Ю.Г.</t>
+          <t>Болвачева И. А.</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>70.66666666666667</v>
+        <v>49.25</v>
       </c>
       <c r="D16" t="n">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="E16" t="n">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F16" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Козлова Е. В.</t>
+          <t>Болотов Г.Е.</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>58.66666666666666</v>
+        <v>59</v>
       </c>
       <c r="D17" t="n">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="E17" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F17" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Колесникова Е,И.</t>
+          <t>Борисов А.Ю.</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>64.33333333333333</v>
+        <v>42.4</v>
       </c>
       <c r="D18" t="n">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="E18" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F18" t="n">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Кондратенко А.Н.</t>
+          <t>Боталов А.М.</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>66.5</v>
+        <v>44.6</v>
       </c>
       <c r="D19" t="n">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="E19" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="F19" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Кузнецов Е.Б.</t>
+          <t>Бубнова Е.В.</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>52.25</v>
+        <v>71</v>
       </c>
       <c r="D20" t="n">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E20" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F20" t="n">
-        <v>66</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Куклина Ф.Н.</t>
+          <t>Будников А.В.</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>211</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+      <c r="F21" t="n">
         <v>52</v>
-      </c>
-      <c r="D21" t="n">
-        <v>156</v>
-      </c>
-      <c r="E21" t="n">
-        <v>38</v>
-      </c>
-      <c r="F21" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Курочкина И.В.</t>
+          <t>Бушуев А.А.</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>61.66666666666666</v>
+        <v>51.5</v>
       </c>
       <c r="D22" t="n">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="E22" t="n">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="F22" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Лобова Е.В.</t>
+          <t>Быков Е.А.</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>65</v>
+        <v>49.2</v>
       </c>
       <c r="D23" t="n">
-        <v>195</v>
+        <v>246</v>
       </c>
       <c r="E23" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="F23" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Макарова А.С.</t>
+          <t>Викторов В.В.</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>104</v>
+        <v>58.5</v>
       </c>
       <c r="D24" t="n">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="E24" t="n">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="F24" t="n">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Марухина Н.А.</t>
+          <t>Вихров Р.Т.</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D25" t="n">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="E25" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F25" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Минкина Е.К.</t>
+          <t>Воробьёв С.В.</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>71</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="D26" t="n">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="E26" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Миронова Л.В.</t>
+          <t>Гавриленко О.В.</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>59.33333333333334</v>
+        <v>50.75</v>
       </c>
       <c r="D27" t="n">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="E27" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F27" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Неустроева С.В.</t>
+          <t>Герасименко А.Т.</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>64</v>
+        <v>40.4</v>
       </c>
       <c r="D28" t="n">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E28" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Нехаев А.В.</t>
+          <t>Горностаев И.Б.</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>69.33333333333333</v>
+        <v>52.33333333333334</v>
       </c>
       <c r="D29" t="n">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="E29" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F29" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Новожилов С.В.</t>
+          <t>Горохова Е.Н.</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>67.66666666666667</v>
+        <v>49</v>
       </c>
       <c r="D30" t="n">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E30" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F30" t="n">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Носова А.А.</t>
+          <t>Гусева Н.И.</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>52.75</v>
+        <v>41.6</v>
       </c>
       <c r="D31" t="n">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E31" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F31" t="n">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Пилатова А.Е. </t>
+          <t>Демидов А.С.</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>48.75</v>
+        <v>59.25</v>
       </c>
       <c r="D32" t="n">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="E32" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F32" t="n">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Ратникова Т.И.</t>
+          <t>Дядищев С.В.</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>48.75</v>
+        <v>43.5</v>
       </c>
       <c r="D33" t="n">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="E33" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F33" t="n">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Сажнева О.В.</t>
+          <t>Ефремов П.С,</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>68.33333333333333</v>
+        <v>50.2</v>
       </c>
       <c r="D34" t="n">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="E34" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F34" t="n">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Силаева О.И.</t>
+          <t>Жукова Г.Б.</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
+        <v>53.25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>213</v>
+      </c>
+      <c r="E35" t="n">
+        <v>45</v>
+      </c>
+      <c r="F35" t="n">
         <v>60</v>
-      </c>
-      <c r="D35" t="n">
-        <v>180</v>
-      </c>
-      <c r="E35" t="n">
-        <v>52</v>
-      </c>
-      <c r="F35" t="n">
-        <v>68</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Смирнова О.В.</t>
+          <t>Захаров Д.И.</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" t="n">
-        <v>65.66666666666667</v>
+        <v>47.4</v>
       </c>
       <c r="D36" t="n">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="E36" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="F36" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Солодовникова Н.В.</t>
+          <t>Захарова К.Г.</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>65.5</v>
+        <v>73</v>
       </c>
       <c r="D37" t="n">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E37" t="n">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F37" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Столярова И.В.</t>
+          <t>Зиновьев С.В.</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>53.66666666666666</v>
+        <v>50.2</v>
       </c>
       <c r="D38" t="n">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="E38" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F38" t="n">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Таковникова Н.А.</t>
+          <t>Инкин Г.А.</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>70.33333333333333</v>
+        <v>46.5</v>
       </c>
       <c r="D39" t="n">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="E39" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="F39" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Тарасова Ю.П.</t>
+          <t>Исаев М.М.</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>56.33333333333334</v>
+        <v>51.25</v>
       </c>
       <c r="D40" t="n">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="E40" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F40" t="n">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Теленкова В.А.</t>
+          <t>Исаева Э.Е.</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>62</v>
+        <v>51.5</v>
       </c>
       <c r="D41" t="n">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="E41" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F41" t="n">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Тихомирова Е.Е.</t>
+          <t>Карева Т.Ю.</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>60.66666666666666</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="D42" t="n">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E42" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F42" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Тришкина Е.В.</t>
+          <t>Киселева Н.В.</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="n">
-        <v>51.5</v>
+        <v>64.33333333333333</v>
       </c>
       <c r="D43" t="n">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="E43" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F43" t="n">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Тушинок С.Н.</t>
+          <t>Кобзев Д.В.</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>66.66666666666667</v>
+        <v>68.66666666666667</v>
       </c>
       <c r="D44" t="n">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E44" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F44" t="n">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Удовенко М.С.</t>
+          <t>Ковалева Ю.Г.</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>64.66666666666667</v>
+        <v>70.66666666666667</v>
       </c>
       <c r="D45" t="n">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="E45" t="n">
         <v>49</v>
       </c>
       <c r="F45" t="n">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Фокина Е.А.</t>
+          <t>Коваленко А.В.</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>49</v>
+        <v>58.25</v>
       </c>
       <c r="D46" t="n">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="E46" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F46" t="n">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Ходченкова М.Н.</t>
+          <t>Козлова Е. В.</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>69.33333333333333</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="D47" t="n">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="E47" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F47" t="n">
         <v>76</v>
@@ -1479,111 +1479,1585 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Христофорова О.С.</t>
+          <t>Колесникова Е,И.</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>3</v>
       </c>
       <c r="C48" t="n">
-        <v>61.33333333333334</v>
+        <v>64.33333333333333</v>
       </c>
       <c r="D48" t="n">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E48" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F48" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Чернявская В.А.</t>
+          <t>Колобков К.М</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C49" t="n">
-        <v>70</v>
+        <v>48.4</v>
       </c>
       <c r="D49" t="n">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="E49" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F49" t="n">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Шварева М.В.</t>
+          <t>Кольцов М.Ю.</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>61.5</v>
+        <v>49.4</v>
       </c>
       <c r="D50" t="n">
-        <v>123</v>
+        <v>247</v>
       </c>
       <c r="E50" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F50" t="n">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Шувалова Т.А.</t>
+          <t>Кондратенко А.Н.</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>42.6</v>
+        <v>66.5</v>
       </c>
       <c r="D51" t="n">
-        <v>213</v>
+        <v>133</v>
       </c>
       <c r="E51" t="n">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="F51" t="n">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
+          <t>Корнеев К.В.</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" t="n">
+        <v>47.25</v>
+      </c>
+      <c r="D52" t="n">
+        <v>189</v>
+      </c>
+      <c r="E52" t="n">
+        <v>35</v>
+      </c>
+      <c r="F52" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>Костин В.Ю.</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="D53" t="n">
+        <v>241</v>
+      </c>
+      <c r="E53" t="n">
+        <v>36</v>
+      </c>
+      <c r="F53" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Костюков Н.В.</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>6</v>
+      </c>
+      <c r="C54" t="n">
+        <v>42.83333333333334</v>
+      </c>
+      <c r="D54" t="n">
+        <v>257</v>
+      </c>
+      <c r="E54" t="n">
+        <v>30</v>
+      </c>
+      <c r="F54" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Кузнецов А.В. </t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="D55" t="n">
+        <v>263</v>
+      </c>
+      <c r="E55" t="n">
+        <v>44</v>
+      </c>
+      <c r="F55" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Кузнецов Е.Б.</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" t="n">
+        <v>52.25</v>
+      </c>
+      <c r="D56" t="n">
+        <v>209</v>
+      </c>
+      <c r="E56" t="n">
+        <v>38</v>
+      </c>
+      <c r="F56" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>Кузьмичев В.К.</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>37</v>
+      </c>
+      <c r="D57" t="n">
+        <v>74</v>
+      </c>
+      <c r="E57" t="n">
+        <v>34</v>
+      </c>
+      <c r="F57" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Куклина Ф.Н.</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C58" t="n">
+        <v>52</v>
+      </c>
+      <c r="D58" t="n">
+        <v>156</v>
+      </c>
+      <c r="E58" t="n">
+        <v>38</v>
+      </c>
+      <c r="F58" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>Курочкина И.В.</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>3</v>
+      </c>
+      <c r="C59" t="n">
+        <v>61.66666666666666</v>
+      </c>
+      <c r="D59" t="n">
+        <v>185</v>
+      </c>
+      <c r="E59" t="n">
+        <v>55</v>
+      </c>
+      <c r="F59" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Лазутин Д.В.</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>48</v>
+      </c>
+      <c r="D60" t="n">
+        <v>240</v>
+      </c>
+      <c r="E60" t="n">
+        <v>37</v>
+      </c>
+      <c r="F60" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>Лобова Е.В.</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>3</v>
+      </c>
+      <c r="C61" t="n">
+        <v>65</v>
+      </c>
+      <c r="D61" t="n">
+        <v>195</v>
+      </c>
+      <c r="E61" t="n">
+        <v>54</v>
+      </c>
+      <c r="F61" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Лыков К.А.</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>6</v>
+      </c>
+      <c r="C62" t="n">
+        <v>43.16666666666666</v>
+      </c>
+      <c r="D62" t="n">
+        <v>259</v>
+      </c>
+      <c r="E62" t="n">
+        <v>30</v>
+      </c>
+      <c r="F62" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>Мазеин А.П.</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="n">
+        <v>42.33333333333334</v>
+      </c>
+      <c r="D63" t="n">
+        <v>254</v>
+      </c>
+      <c r="E63" t="n">
+        <v>37</v>
+      </c>
+      <c r="F63" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>Макарова А.С.</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>104</v>
+      </c>
+      <c r="D64" t="n">
+        <v>208</v>
+      </c>
+      <c r="E64" t="n">
+        <v>100</v>
+      </c>
+      <c r="F64" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>Марухина Н.А.</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>53</v>
+      </c>
+      <c r="D65" t="n">
+        <v>159</v>
+      </c>
+      <c r="E65" t="n">
+        <v>41</v>
+      </c>
+      <c r="F65" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Медведев П.С.</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>4</v>
+      </c>
+      <c r="C66" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="D66" t="n">
+        <v>222</v>
+      </c>
+      <c r="E66" t="n">
+        <v>44</v>
+      </c>
+      <c r="F66" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>Минкина Е.К.</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" t="n">
+        <v>78</v>
+      </c>
+      <c r="D67" t="n">
+        <v>78</v>
+      </c>
+      <c r="E67" t="n">
+        <v>78</v>
+      </c>
+      <c r="F67" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Миронова Л.В.</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="n">
+        <v>59.33333333333334</v>
+      </c>
+      <c r="D68" t="n">
+        <v>178</v>
+      </c>
+      <c r="E68" t="n">
+        <v>40</v>
+      </c>
+      <c r="F68" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Мурзак Д.Г.</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>4</v>
+      </c>
+      <c r="C69" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="D69" t="n">
+        <v>234</v>
+      </c>
+      <c r="E69" t="n">
+        <v>48</v>
+      </c>
+      <c r="F69" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>Мусин Р.М.</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="D70" t="n">
+        <v>234</v>
+      </c>
+      <c r="E70" t="n">
+        <v>48</v>
+      </c>
+      <c r="F70" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>Наротьев М.А.</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>3</v>
+      </c>
+      <c r="C71" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="D71" t="n">
+        <v>133</v>
+      </c>
+      <c r="E71" t="n">
+        <v>33</v>
+      </c>
+      <c r="F71" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>Неустроева С.В.</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C72" t="n">
+        <v>64</v>
+      </c>
+      <c r="D72" t="n">
+        <v>192</v>
+      </c>
+      <c r="E72" t="n">
+        <v>59</v>
+      </c>
+      <c r="F72" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>Нехаев А.В.</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3</v>
+      </c>
+      <c r="C73" t="n">
+        <v>69.33333333333333</v>
+      </c>
+      <c r="D73" t="n">
+        <v>208</v>
+      </c>
+      <c r="E73" t="n">
+        <v>58</v>
+      </c>
+      <c r="F73" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Нижневский П.А.</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>3</v>
+      </c>
+      <c r="C74" t="n">
+        <v>40</v>
+      </c>
+      <c r="D74" t="n">
+        <v>120</v>
+      </c>
+      <c r="E74" t="n">
+        <v>34</v>
+      </c>
+      <c r="F74" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Новожилов С.В.</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="n">
+        <v>67.66666666666667</v>
+      </c>
+      <c r="D75" t="n">
+        <v>203</v>
+      </c>
+      <c r="E75" t="n">
+        <v>46</v>
+      </c>
+      <c r="F75" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Ноздряков М.С</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2</v>
+      </c>
+      <c r="C76" t="n">
+        <v>70</v>
+      </c>
+      <c r="D76" t="n">
+        <v>140</v>
+      </c>
+      <c r="E76" t="n">
+        <v>61</v>
+      </c>
+      <c r="F76" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Носова А.А.</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>4</v>
+      </c>
+      <c r="C77" t="n">
+        <v>52.75</v>
+      </c>
+      <c r="D77" t="n">
+        <v>211</v>
+      </c>
+      <c r="E77" t="n">
+        <v>40</v>
+      </c>
+      <c r="F77" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Павленко Г.Е.</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="D78" t="n">
+        <v>243</v>
+      </c>
+      <c r="E78" t="n">
+        <v>34</v>
+      </c>
+      <c r="F78" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Першин А.А.</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>4</v>
+      </c>
+      <c r="C79" t="n">
+        <v>60</v>
+      </c>
+      <c r="D79" t="n">
+        <v>240</v>
+      </c>
+      <c r="E79" t="n">
+        <v>32</v>
+      </c>
+      <c r="F79" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Пилатова А.Е. </t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="D80" t="n">
+        <v>195</v>
+      </c>
+      <c r="E80" t="n">
+        <v>28</v>
+      </c>
+      <c r="F80" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Ратникова Т.И.</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>4</v>
+      </c>
+      <c r="C81" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="D81" t="n">
+        <v>195</v>
+      </c>
+      <c r="E81" t="n">
+        <v>34</v>
+      </c>
+      <c r="F81" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Савченко А.В.</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="D82" t="n">
+        <v>251</v>
+      </c>
+      <c r="E82" t="n">
+        <v>41</v>
+      </c>
+      <c r="F82" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Садов К.К.</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>3</v>
+      </c>
+      <c r="C83" t="n">
+        <v>62.33333333333334</v>
+      </c>
+      <c r="D83" t="n">
+        <v>187</v>
+      </c>
+      <c r="E83" t="n">
+        <v>44</v>
+      </c>
+      <c r="F83" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Сажнева О.В.</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="n">
+        <v>68.33333333333333</v>
+      </c>
+      <c r="D84" t="n">
+        <v>205</v>
+      </c>
+      <c r="E84" t="n">
+        <v>49</v>
+      </c>
+      <c r="F84" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Свечников В.В.</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>4</v>
+      </c>
+      <c r="C85" t="n">
+        <v>66</v>
+      </c>
+      <c r="D85" t="n">
+        <v>264</v>
+      </c>
+      <c r="E85" t="n">
+        <v>48</v>
+      </c>
+      <c r="F85" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Серухин А.В.</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>6</v>
+      </c>
+      <c r="C86" t="n">
+        <v>43.66666666666666</v>
+      </c>
+      <c r="D86" t="n">
+        <v>262</v>
+      </c>
+      <c r="E86" t="n">
+        <v>30</v>
+      </c>
+      <c r="F86" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Силаева О.И.</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" t="n">
+        <v>60</v>
+      </c>
+      <c r="D87" t="n">
+        <v>180</v>
+      </c>
+      <c r="E87" t="n">
+        <v>52</v>
+      </c>
+      <c r="F87" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Синяков А.В.</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>2</v>
+      </c>
+      <c r="C88" t="n">
+        <v>37</v>
+      </c>
+      <c r="D88" t="n">
+        <v>74</v>
+      </c>
+      <c r="E88" t="n">
+        <v>34</v>
+      </c>
+      <c r="F88" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Сироткин А.Н.</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" t="n">
+        <v>42</v>
+      </c>
+      <c r="D89" t="n">
+        <v>126</v>
+      </c>
+      <c r="E89" t="n">
+        <v>39</v>
+      </c>
+      <c r="F89" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Скрябин С.Н.</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>74.66666666666667</v>
+      </c>
+      <c r="D90" t="n">
+        <v>224</v>
+      </c>
+      <c r="E90" t="n">
+        <v>48</v>
+      </c>
+      <c r="F90" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Смирнова О.В.</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" t="n">
+        <v>65.66666666666667</v>
+      </c>
+      <c r="D91" t="n">
+        <v>197</v>
+      </c>
+      <c r="E91" t="n">
+        <v>53</v>
+      </c>
+      <c r="F91" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>Солодовникова Н.В.</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>2</v>
+      </c>
+      <c r="C92" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="D92" t="n">
+        <v>131</v>
+      </c>
+      <c r="E92" t="n">
+        <v>61</v>
+      </c>
+      <c r="F92" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Солтан Д. С.</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="D93" t="n">
+        <v>256</v>
+      </c>
+      <c r="E93" t="n">
+        <v>37</v>
+      </c>
+      <c r="F93" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Столярова И.В.</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" t="n">
+        <v>58.66666666666666</v>
+      </c>
+      <c r="D94" t="n">
+        <v>176</v>
+      </c>
+      <c r="E94" t="n">
+        <v>56</v>
+      </c>
+      <c r="F94" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Таковникова Н.А.</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>3</v>
+      </c>
+      <c r="C95" t="n">
+        <v>70.33333333333333</v>
+      </c>
+      <c r="D95" t="n">
+        <v>211</v>
+      </c>
+      <c r="E95" t="n">
+        <v>61</v>
+      </c>
+      <c r="F95" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Тарасова Ю.П.</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>3</v>
+      </c>
+      <c r="C96" t="n">
+        <v>56.33333333333334</v>
+      </c>
+      <c r="D96" t="n">
+        <v>169</v>
+      </c>
+      <c r="E96" t="n">
+        <v>48</v>
+      </c>
+      <c r="F96" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Теленкова В.А.</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>3</v>
+      </c>
+      <c r="C97" t="n">
+        <v>62</v>
+      </c>
+      <c r="D97" t="n">
+        <v>186</v>
+      </c>
+      <c r="E97" t="n">
+        <v>45</v>
+      </c>
+      <c r="F97" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Тимонин А.В.</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>6</v>
+      </c>
+      <c r="C98" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="D98" t="n">
+        <v>266</v>
+      </c>
+      <c r="E98" t="n">
+        <v>31</v>
+      </c>
+      <c r="F98" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Тихомирова Е.Е.</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>3</v>
+      </c>
+      <c r="C99" t="n">
+        <v>60.66666666666666</v>
+      </c>
+      <c r="D99" t="n">
+        <v>182</v>
+      </c>
+      <c r="E99" t="n">
+        <v>48</v>
+      </c>
+      <c r="F99" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Тришкина Е.В.</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>4</v>
+      </c>
+      <c r="C100" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="D100" t="n">
+        <v>206</v>
+      </c>
+      <c r="E100" t="n">
+        <v>47</v>
+      </c>
+      <c r="F100" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Тушинок С.Н.</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>2</v>
+      </c>
+      <c r="C101" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="D101" t="n">
+        <v>129</v>
+      </c>
+      <c r="E101" t="n">
+        <v>62</v>
+      </c>
+      <c r="F101" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Удовенко М.С.</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C102" t="n">
+        <v>64.66666666666667</v>
+      </c>
+      <c r="D102" t="n">
+        <v>194</v>
+      </c>
+      <c r="E102" t="n">
+        <v>49</v>
+      </c>
+      <c r="F102" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Уткин Н.С.</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>5</v>
+      </c>
+      <c r="C103" t="n">
+        <v>53.4</v>
+      </c>
+      <c r="D103" t="n">
+        <v>267</v>
+      </c>
+      <c r="E103" t="n">
+        <v>41</v>
+      </c>
+      <c r="F103" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Филиппов В.М.</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>5</v>
+      </c>
+      <c r="C104" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="D104" t="n">
+        <v>232</v>
+      </c>
+      <c r="E104" t="n">
+        <v>37</v>
+      </c>
+      <c r="F104" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Фокина Е.А.</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>4</v>
+      </c>
+      <c r="C105" t="n">
+        <v>49</v>
+      </c>
+      <c r="D105" t="n">
+        <v>196</v>
+      </c>
+      <c r="E105" t="n">
+        <v>32</v>
+      </c>
+      <c r="F105" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Фролов К.В.</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" t="n">
+        <v>79</v>
+      </c>
+      <c r="D106" t="n">
+        <v>79</v>
+      </c>
+      <c r="E106" t="n">
+        <v>79</v>
+      </c>
+      <c r="F106" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Хализев В.И.</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>3</v>
+      </c>
+      <c r="C107" t="n">
+        <v>44.33333333333334</v>
+      </c>
+      <c r="D107" t="n">
+        <v>133</v>
+      </c>
+      <c r="E107" t="n">
+        <v>33</v>
+      </c>
+      <c r="F107" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Ходорко В.Э.</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>5</v>
+      </c>
+      <c r="C108" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="D108" t="n">
+        <v>241</v>
+      </c>
+      <c r="E108" t="n">
+        <v>31</v>
+      </c>
+      <c r="F108" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>Ходченкова М.Н.</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>3</v>
+      </c>
+      <c r="C109" t="n">
+        <v>69.33333333333333</v>
+      </c>
+      <c r="D109" t="n">
+        <v>208</v>
+      </c>
+      <c r="E109" t="n">
+        <v>65</v>
+      </c>
+      <c r="F109" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Христофорова О.С.</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>3</v>
+      </c>
+      <c r="C110" t="n">
+        <v>61.33333333333334</v>
+      </c>
+      <c r="D110" t="n">
+        <v>184</v>
+      </c>
+      <c r="E110" t="n">
+        <v>52</v>
+      </c>
+      <c r="F110" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Цыбаков С.Ю</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>5</v>
+      </c>
+      <c r="C111" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="D111" t="n">
+        <v>249</v>
+      </c>
+      <c r="E111" t="n">
+        <v>32</v>
+      </c>
+      <c r="F111" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Чернявская В.А.</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>3</v>
+      </c>
+      <c r="C112" t="n">
+        <v>70</v>
+      </c>
+      <c r="D112" t="n">
+        <v>210</v>
+      </c>
+      <c r="E112" t="n">
+        <v>43</v>
+      </c>
+      <c r="F112" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Шарфутов А.В.</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>2</v>
+      </c>
+      <c r="C113" t="n">
+        <v>40</v>
+      </c>
+      <c r="D113" t="n">
+        <v>80</v>
+      </c>
+      <c r="E113" t="n">
+        <v>40</v>
+      </c>
+      <c r="F113" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>Шварева М.В.</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>2</v>
+      </c>
+      <c r="C114" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>123</v>
+      </c>
+      <c r="E114" t="n">
+        <v>50</v>
+      </c>
+      <c r="F114" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Шейман И.Г.</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>6</v>
+      </c>
+      <c r="C115" t="n">
+        <v>40.83333333333334</v>
+      </c>
+      <c r="D115" t="n">
+        <v>245</v>
+      </c>
+      <c r="E115" t="n">
+        <v>30</v>
+      </c>
+      <c r="F115" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>Шипунов А.В.</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>5</v>
+      </c>
+      <c r="C116" t="n">
+        <v>54.2</v>
+      </c>
+      <c r="D116" t="n">
+        <v>271</v>
+      </c>
+      <c r="E116" t="n">
+        <v>37</v>
+      </c>
+      <c r="F116" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Шувалова Т.А.</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>5</v>
+      </c>
+      <c r="C117" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="D117" t="n">
+        <v>213</v>
+      </c>
+      <c r="E117" t="n">
+        <v>25</v>
+      </c>
+      <c r="F117" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
           <t>Шуйкова С.М.</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>3</v>
-      </c>
-      <c r="C52" t="n">
+      <c r="B118" t="n">
+        <v>3</v>
+      </c>
+      <c r="C118" t="n">
         <v>64.33333333333333</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D118" t="n">
         <v>193</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E118" t="n">
         <v>54</v>
       </c>
-      <c r="F52" t="n">
+      <c r="F118" t="n">
         <v>74</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>Щедрин М.А.</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>5</v>
+      </c>
+      <c r="C119" t="n">
+        <v>53</v>
+      </c>
+      <c r="D119" t="n">
+        <v>265</v>
+      </c>
+      <c r="E119" t="n">
+        <v>41</v>
+      </c>
+      <c r="F119" t="n">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>